<commit_message>
Disable seeds as agreed in CMSHLT-3145
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2024_v1_0_0/PrescaleTable/L1Menu_Collisions2024_v1_0_0.xlsx
+++ b/official/L1Menu_Collisions2024_v1_0_0/PrescaleTable/L1Menu_Collisions2024_v1_0_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2024_v1_0_0/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-master 24/official/L1Menu_Collisions2024_v1_0_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4E62E7-5245-9E42-9E31-BABD1269BAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B1846E-E94A-A245-ABC1-76803684ADF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10180" yWindow="-19560" windowWidth="30400" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="1320" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1637,8 +1637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A328" workbookViewId="0">
-      <selection activeCell="B356" sqref="B356"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10351,82 +10351,82 @@
       <c r="A213">
         <v>239</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B213" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C213">
-        <v>0</v>
-      </c>
-      <c r="D213">
-        <v>1</v>
-      </c>
-      <c r="E213">
-        <v>1</v>
-      </c>
-      <c r="F213">
-        <v>1</v>
-      </c>
-      <c r="G213">
-        <v>1</v>
-      </c>
-      <c r="H213">
-        <v>1</v>
-      </c>
-      <c r="I213">
-        <v>1</v>
-      </c>
-      <c r="J213">
-        <v>1</v>
+      <c r="C213" s="1">
+        <v>0</v>
+      </c>
+      <c r="D213" s="1">
+        <v>0</v>
+      </c>
+      <c r="E213" s="1">
+        <v>0</v>
+      </c>
+      <c r="F213" s="1">
+        <v>0</v>
+      </c>
+      <c r="G213" s="1">
+        <v>0</v>
+      </c>
+      <c r="H213" s="1">
+        <v>0</v>
+      </c>
+      <c r="I213" s="1">
+        <v>0</v>
+      </c>
+      <c r="J213" s="1">
+        <v>0</v>
       </c>
       <c r="K213" s="1">
         <v>0</v>
       </c>
-      <c r="L213">
-        <v>1</v>
-      </c>
-      <c r="M213">
-        <v>1</v>
+      <c r="L213" s="1">
+        <v>0</v>
+      </c>
+      <c r="M213" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>240</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C214">
-        <v>0</v>
-      </c>
-      <c r="D214">
-        <v>1</v>
-      </c>
-      <c r="E214">
-        <v>1</v>
-      </c>
-      <c r="F214">
-        <v>1</v>
-      </c>
-      <c r="G214">
-        <v>1</v>
-      </c>
-      <c r="H214">
-        <v>1</v>
-      </c>
-      <c r="I214">
-        <v>1</v>
-      </c>
-      <c r="J214">
-        <v>1</v>
+      <c r="C214" s="1">
+        <v>0</v>
+      </c>
+      <c r="D214" s="1">
+        <v>0</v>
+      </c>
+      <c r="E214" s="1">
+        <v>0</v>
+      </c>
+      <c r="F214" s="1">
+        <v>0</v>
+      </c>
+      <c r="G214" s="1">
+        <v>0</v>
+      </c>
+      <c r="H214" s="1">
+        <v>0</v>
+      </c>
+      <c r="I214" s="1">
+        <v>0</v>
+      </c>
+      <c r="J214" s="1">
+        <v>0</v>
       </c>
       <c r="K214" s="1">
         <v>0</v>
       </c>
-      <c r="L214">
-        <v>1</v>
-      </c>
-      <c r="M214">
-        <v>1</v>
+      <c r="L214" s="1">
+        <v>0</v>
+      </c>
+      <c r="M214" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.2">
@@ -10597,41 +10597,41 @@
       <c r="A219">
         <v>245</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B219" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C219">
-        <v>0</v>
-      </c>
-      <c r="D219">
-        <v>1</v>
-      </c>
-      <c r="E219">
-        <v>1</v>
-      </c>
-      <c r="F219">
-        <v>1</v>
-      </c>
-      <c r="G219">
-        <v>1</v>
-      </c>
-      <c r="H219">
-        <v>1</v>
-      </c>
-      <c r="I219">
-        <v>1</v>
-      </c>
-      <c r="J219">
-        <v>1</v>
+      <c r="C219" s="1">
+        <v>0</v>
+      </c>
+      <c r="D219" s="1">
+        <v>0</v>
+      </c>
+      <c r="E219" s="1">
+        <v>0</v>
+      </c>
+      <c r="F219" s="1">
+        <v>0</v>
+      </c>
+      <c r="G219" s="1">
+        <v>0</v>
+      </c>
+      <c r="H219" s="1">
+        <v>0</v>
+      </c>
+      <c r="I219" s="1">
+        <v>0</v>
+      </c>
+      <c r="J219" s="1">
+        <v>0</v>
       </c>
       <c r="K219" s="1">
         <v>0</v>
       </c>
-      <c r="L219">
-        <v>1</v>
-      </c>
-      <c r="M219">
-        <v>1</v>
+      <c r="L219" s="1">
+        <v>0</v>
+      </c>
+      <c r="M219" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>